<commit_message>
Some fixes in DB homeworks
</commit_message>
<xml_diff>
--- a/SoftwareTechnoligies/DataBases/07. ADO.Net/ADO.Net/ReadExcelFile/myWorksheet.xlsx
+++ b/SoftwareTechnoligies/DataBases/07. ADO.Net/ADO.Net/ReadExcelFile/myWorksheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -534,18 +534,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" rightToLeft="false"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row spans="1:2" outlineLevel="0" r="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row spans="1:2" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -561,7 +561,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row spans="1:2" outlineLevel="0" r="3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -569,7 +569,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row spans="1:2" outlineLevel="0" r="4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -577,12 +577,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row spans="1:2" outlineLevel="0" r="5">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="6">
         <v>20</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>Pesho</t>
+        </is>
+      </c>
+      <c r="B6" s="6">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean up SoftwareTechnoligies folder
</commit_message>
<xml_diff>
--- a/SoftwareTechnoligies/DataBases/07. ADO.Net/ADO.Net/ReadExcelFile/myWorksheet.xlsx
+++ b/SoftwareTechnoligies/DataBases/07. ADO.Net/ADO.Net/ReadExcelFile/myWorksheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="true"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
@@ -534,18 +534,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" rightToLeft="false"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:2" outlineLevel="0" r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row spans="1:2" outlineLevel="0" r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -561,7 +561,7 @@
         <v>25</v>
       </c>
     </row>
-    <row spans="1:2" outlineLevel="0" r="3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -569,7 +569,7 @@
         <v>22</v>
       </c>
     </row>
-    <row spans="1:2" outlineLevel="0" r="4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -577,22 +577,12 @@
         <v>24</v>
       </c>
     </row>
-    <row spans="1:2" outlineLevel="0" r="5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="6">
         <v>20</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="6">
-      <c r="A6" s="6" t="inlineStr">
-        <is>
-          <t>Pesho</t>
-        </is>
-      </c>
-      <c r="B6" s="6">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>